<commit_message>
Upload updated documentation and files
</commit_message>
<xml_diff>
--- a/Bom Lists/myCPU_Full_BOM_List.xlsx
+++ b/Bom Lists/myCPU_Full_BOM_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unedo365-my.sharepoint.com/personal/rhernande522_alumno_uned_es/Documents/Projects/Altium/myCPU/#Documents/BOM Files/Full BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="631" documentId="8_{D68AE115-F819-4B31-904E-9CCC2262B984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{104201B3-E2F6-44B1-9278-06126A73418C}"/>
+  <xr:revisionPtr revIDLastSave="638" documentId="8_{D68AE115-F819-4B31-904E-9CCC2262B984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CB3EB00-B731-496F-B37F-2DFBCF0C6730}"/>
   <bookViews>
-    <workbookView xWindow="16965" yWindow="195" windowWidth="16260" windowHeight="14475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="1200" windowWidth="28185" windowHeight="13965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICs" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Wire" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Components!$A$1:$C$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Components!$A$1:$C$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Connectors!$A$1:$C$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ICs!$A$1:$C$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Wire!$A$1:$C$13</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
   <si>
     <t>Description</t>
   </si>
@@ -379,13 +379,16 @@
     <t>220µF</t>
   </si>
   <si>
-    <t>7805 Voltage Regulator 5v / 1A</t>
-  </si>
-  <si>
     <t>LM7805</t>
   </si>
   <si>
-    <t>HeatSink for the 7805 14x18x10</t>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>7805 Voltage Regulator 5v / 1A TO-220F isolated</t>
+  </si>
+  <si>
+    <t>HeatSink for the 7805 14x18x10 mm or 14x18x6 mm</t>
   </si>
 </sst>
 </file>
@@ -1477,8 +1480,8 @@
   </sheetPr>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2176,10 +2179,10 @@
     </row>
     <row r="31" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="33" t="s">
         <v>116</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>117</v>
       </c>
       <c r="C31" s="27">
         <v>10</v>
@@ -2553,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO54"/>
+  <dimension ref="A1:AO55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3446,14 +3449,14 @@
       <c r="AO25" s="20"/>
     </row>
     <row r="26" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="10">
-        <v>1</v>
+      <c r="B26" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3495,14 +3498,14 @@
       <c r="AO26" s="20"/>
     </row>
     <row r="27" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="8">
-        <v>12</v>
+      <c r="B27" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="10">
+        <v>1</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -3548,10 +3551,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C28" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3593,14 +3596,14 @@
       <c r="AO28" s="20"/>
     </row>
     <row r="29" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>52</v>
+      <c r="A29" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C29" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3646,10 +3649,10 @@
         <v>52</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="8">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
@@ -3691,14 +3694,14 @@
       <c r="AO30" s="20"/>
     </row>
     <row r="31" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>15</v>
+      <c r="A31" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C31" s="8">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -3740,14 +3743,14 @@
       <c r="AO31" s="20"/>
     </row>
     <row r="32" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>95</v>
+      <c r="A32" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C32" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
@@ -3788,67 +3791,67 @@
       <c r="AN32" s="20"/>
       <c r="AO32" s="20"/>
     </row>
-    <row r="33" spans="1:41" s="42" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-    </row>
-    <row r="34" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+    <row r="33" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="8">
+        <v>4</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="20"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="20"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="20"/>
+      <c r="AE33" s="20"/>
+      <c r="AF33" s="20"/>
+      <c r="AG33" s="20"/>
+      <c r="AH33" s="20"/>
+      <c r="AI33" s="20"/>
+      <c r="AJ33" s="20"/>
+      <c r="AK33" s="20"/>
+      <c r="AL33" s="20"/>
+      <c r="AM33" s="20"/>
+      <c r="AN33" s="20"/>
+      <c r="AO33" s="20"/>
+    </row>
+    <row r="34" spans="1:41" s="42" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+    </row>
+    <row r="35" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B35" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="8">
-        <v>2</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
-      <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
-      <c r="Y34" s="20"/>
-      <c r="Z34" s="20"/>
-      <c r="AA34" s="20"/>
-      <c r="AB34" s="20"/>
-      <c r="AC34" s="20"/>
-      <c r="AD34" s="20"/>
-      <c r="AE34" s="20"/>
-      <c r="AF34" s="20"/>
-      <c r="AG34" s="20"/>
-      <c r="AH34" s="20"/>
-      <c r="AI34" s="20"/>
-      <c r="AJ34" s="20"/>
-      <c r="AK34" s="20"/>
-      <c r="AL34" s="20"/>
-      <c r="AM34" s="20"/>
-      <c r="AN34" s="20"/>
-      <c r="AO34" s="20"/>
-    </row>
-    <row r="35" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="10">
+      <c r="C35" s="8">
         <v>2</v>
       </c>
       <c r="D35" s="20"/>
@@ -3892,13 +3895,13 @@
     </row>
     <row r="36" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C36" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
@@ -3941,11 +3944,13 @@
     </row>
     <row r="37" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="34"/>
+        <v>10</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>102</v>
+      </c>
       <c r="C37" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -3987,12 +3992,12 @@
       <c r="AO37" s="20"/>
     </row>
     <row r="38" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="14">
-        <v>2</v>
+      <c r="A38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="10">
+        <v>5</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -4033,64 +4038,62 @@
       <c r="AN38" s="20"/>
       <c r="AO38" s="20"/>
     </row>
-    <row r="39" spans="1:41" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="28">
-        <v>3</v>
-      </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="21"/>
-      <c r="AC39" s="21"/>
-      <c r="AD39" s="21"/>
-      <c r="AE39" s="21"/>
-      <c r="AF39" s="21"/>
-      <c r="AG39" s="21"/>
-      <c r="AH39" s="21"/>
-      <c r="AI39" s="21"/>
-      <c r="AJ39" s="21"/>
-      <c r="AK39" s="21"/>
-      <c r="AL39" s="21"/>
-      <c r="AM39" s="21"/>
-      <c r="AN39" s="21"/>
-      <c r="AO39" s="21"/>
+    <row r="39" spans="1:41" s="19" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="14">
+        <v>2</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="20"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="20"/>
+      <c r="AM39" s="20"/>
+      <c r="AN39" s="20"/>
+      <c r="AO39" s="20"/>
     </row>
     <row r="40" spans="1:41" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C40" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
@@ -4136,10 +4139,10 @@
         <v>55</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
@@ -4181,12 +4184,14 @@
       <c r="AO41" s="21"/>
     </row>
     <row r="42" spans="1:41" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="37"/>
+      <c r="A42" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>61</v>
+      </c>
       <c r="C42" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
@@ -4228,9 +4233,13 @@
       <c r="AO42" s="21"/>
     </row>
     <row r="43" spans="1:41" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
+      <c r="A43" s="25" t="s">
+        <v>119</v>
+      </c>
       <c r="B43" s="37"/>
-      <c r="C43" s="28"/>
+      <c r="C43" s="28">
+        <v>10</v>
+      </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
@@ -4485,48 +4494,48 @@
       <c r="AN48" s="21"/>
       <c r="AO48" s="21"/>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
+    <row r="49" spans="1:41" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25"/>
       <c r="B49" s="37"/>
       <c r="C49" s="28"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="15"/>
-      <c r="AA49" s="15"/>
-      <c r="AB49" s="15"/>
-      <c r="AC49" s="15"/>
-      <c r="AD49" s="15"/>
-      <c r="AE49" s="15"/>
-      <c r="AF49" s="15"/>
-      <c r="AG49" s="15"/>
-      <c r="AH49" s="15"/>
-      <c r="AI49" s="15"/>
-      <c r="AJ49" s="15"/>
-      <c r="AK49" s="15"/>
-      <c r="AL49" s="15"/>
-      <c r="AM49" s="15"/>
-      <c r="AN49" s="15"/>
-      <c r="AO49" s="15"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="21"/>
+      <c r="U49" s="21"/>
+      <c r="V49" s="21"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
+      <c r="AA49" s="21"/>
+      <c r="AB49" s="21"/>
+      <c r="AC49" s="21"/>
+      <c r="AD49" s="21"/>
+      <c r="AE49" s="21"/>
+      <c r="AF49" s="21"/>
+      <c r="AG49" s="21"/>
+      <c r="AH49" s="21"/>
+      <c r="AI49" s="21"/>
+      <c r="AJ49" s="21"/>
+      <c r="AK49" s="21"/>
+      <c r="AL49" s="21"/>
+      <c r="AM49" s="21"/>
+      <c r="AN49" s="21"/>
+      <c r="AO49" s="21"/>
     </row>
     <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
@@ -4743,6 +4752,49 @@
       <c r="AN54" s="15"/>
       <c r="AO54" s="15"/>
     </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="15"/>
+      <c r="U55" s="15"/>
+      <c r="V55" s="15"/>
+      <c r="W55" s="15"/>
+      <c r="X55" s="15"/>
+      <c r="Y55" s="15"/>
+      <c r="Z55" s="15"/>
+      <c r="AA55" s="15"/>
+      <c r="AB55" s="15"/>
+      <c r="AC55" s="15"/>
+      <c r="AD55" s="15"/>
+      <c r="AE55" s="15"/>
+      <c r="AF55" s="15"/>
+      <c r="AG55" s="15"/>
+      <c r="AH55" s="15"/>
+      <c r="AI55" s="15"/>
+      <c r="AJ55" s="15"/>
+      <c r="AK55" s="15"/>
+      <c r="AL55" s="15"/>
+      <c r="AM55" s="15"/>
+      <c r="AN55" s="15"/>
+      <c r="AO55" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C5"/>
@@ -4763,7 +4815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2909180E-E544-4798-A06A-E19338938FB9}">
   <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>